<commit_message>
Results with more cores
</commit_message>
<xml_diff>
--- a/src/main/org/deidentifier/arx/distributed/eval.xlsx
+++ b/src/main/org/deidentifier/arx/distributed/eval.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mail\git\arx\src\main\org\deidentifier\arx\distribution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mail\git\arx\src\main\org\deidentifier\arx\distributed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC9BC9C-83F3-4BBF-9378-4D0B81698121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69451CB-DC68-4257-B5AA-5DAD50D6602A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2207E27C-B32F-4C7E-B1A0-3C25600B901E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="6">
   <si>
     <t>Threads</t>
   </si>
@@ -41,7 +41,16 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Quality</t>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>Granularity</t>
+  </si>
+  <si>
+    <t>Ihis</t>
   </si>
 </sst>
 </file>
@@ -131,7 +140,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Sorted Partitioning</a:t>
+              <a:t>Sorted Partitioning (k=5)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -172,97 +181,15 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$D$2</c:f>
+              <c:f>Tabelle1!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>Time</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$D$3:$D$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>67867</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>48195</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43720</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>39445</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-52E6-46B8-9A34-5220990A28C8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1024859584"/>
-        <c:axId val="1024860000"/>
-      </c:lineChart>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Quality</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -293,21 +220,72 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$3:$C$6</c:f>
+              <c:f>Tabelle1!$F$4:$F$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.96763307859054104</c:v>
+                  <c:v>66692</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.96254847707062496</c:v>
+                  <c:v>33353</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95707787789263299</c:v>
+                  <c:v>26131</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.95719143086468705</c:v>
+                  <c:v>18826</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16914</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16379</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15707</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12102</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11913</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12144</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9794</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10305</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8746</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9771</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8459</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8095</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8347</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7453</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7452</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7297</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7370</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -315,7 +293,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-52E6-46B8-9A34-5220990A28C8}"/>
+              <c16:uniqueId val="{00000001-91F0-4852-9A23-AACE878B67D3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -329,8 +307,141 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1023909856"/>
-        <c:axId val="1023911936"/>
+        <c:axId val="1024859584"/>
+        <c:axId val="1024860000"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Granularity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$E$4:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.96763307859054104</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96254847707062496</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95707787789263299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95719143086468705</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.951799211415157</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95044550661094895</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94910406910980505</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.94631494771818903</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.94176747817304696</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.94097541924430705</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.93946599857246005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.93912039244564605</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.93891405303633901</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.93696775706535096</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.93704761416094795</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.93679578101456695</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.93665483908422498</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.935996256544808</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.93521532397336504</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.93508554720051995</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.933773849746796</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-91F0-4852-9A23-AACE878B67D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="720937760"/>
+        <c:axId val="720951072"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="1024859584"/>
@@ -439,7 +550,7 @@
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1023911936"/>
+        <c:axId val="720951072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -447,7 +558,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
-        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -478,12 +589,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1023909856"/>
+        <c:crossAx val="720937760"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1023909856"/>
+        <c:axId val="720937760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -492,7 +603,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1023911936"/>
+        <c:crossAx val="720951072"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1128,16 +1239,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1462,67 +1573,386 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908B8DC0-A531-437E-9555-E46366EDC663}">
-  <dimension ref="B2:D6"/>
+  <dimension ref="B3:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0.96763307859054104</v>
+      </c>
+      <c r="F4">
+        <v>66692</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>0.96763307859054104</v>
-      </c>
-      <c r="D3">
-        <v>67867</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
+      <c r="E5">
         <v>0.96254847707062496</v>
       </c>
-      <c r="D4">
-        <v>48195</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="F5">
+        <v>33353</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="E6">
         <v>0.95707787789263299</v>
       </c>
-      <c r="D5">
-        <v>43720</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="F6">
+        <v>26131</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="E7">
         <v>0.95719143086468705</v>
       </c>
-      <c r="D6">
-        <v>39445</v>
+      <c r="F7">
+        <v>18826</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>0.951799211415157</v>
+      </c>
+      <c r="F8">
+        <v>16914</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>0.95044550661094895</v>
+      </c>
+      <c r="F9">
+        <v>16379</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>0.94910406910980505</v>
+      </c>
+      <c r="F10">
+        <v>15707</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>0.94631494771818903</v>
+      </c>
+      <c r="F11">
+        <v>12102</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>0.94176747817304696</v>
+      </c>
+      <c r="F12">
+        <v>11913</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>0.94097541924430705</v>
+      </c>
+      <c r="F13">
+        <v>12144</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>0.93946599857246005</v>
+      </c>
+      <c r="F14">
+        <v>9794</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <v>0.93912039244564605</v>
+      </c>
+      <c r="F15">
+        <v>10305</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>13</v>
+      </c>
+      <c r="E16">
+        <v>0.93891405303633901</v>
+      </c>
+      <c r="F16">
+        <v>8746</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>14</v>
+      </c>
+      <c r="E17">
+        <v>0.93696775706535096</v>
+      </c>
+      <c r="F17">
+        <v>9771</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>0.93704761416094795</v>
+      </c>
+      <c r="F18">
+        <v>8459</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <v>0.93679578101456695</v>
+      </c>
+      <c r="F19">
+        <v>8095</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>17</v>
+      </c>
+      <c r="E20">
+        <v>0.93665483908422498</v>
+      </c>
+      <c r="F20">
+        <v>8347</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>18</v>
+      </c>
+      <c r="E21">
+        <v>0.935996256544808</v>
+      </c>
+      <c r="F21">
+        <v>7453</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>19</v>
+      </c>
+      <c r="E22">
+        <v>0.93521532397336504</v>
+      </c>
+      <c r="F22">
+        <v>7452</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>20</v>
+      </c>
+      <c r="E23">
+        <v>0.93508554720051995</v>
+      </c>
+      <c r="F23">
+        <v>7297</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>21</v>
+      </c>
+      <c r="E24">
+        <v>0.933773849746796</v>
+      </c>
+      <c r="F24">
+        <v>7370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add results for differential privay
</commit_message>
<xml_diff>
--- a/src/main/org/deidentifier/arx/distributed/eval.xlsx
+++ b/src/main/org/deidentifier/arx/distributed/eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mail\git\arx\src\main\org\deidentifier\arx\distributed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F1DE13-5232-4940-AFF4-C29D73F657AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101AA411-EF58-4EF4-8362-73D3CA391E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2207E27C-B32F-4C7E-B1A0-3C25600B901E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2207E27C-B32F-4C7E-B1A0-3C25600B901E}"/>
   </bookViews>
   <sheets>
     <sheet name="Local" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6838" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7101" uniqueCount="24">
   <si>
     <t>Threads</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>0,01-average-risk</t>
+  </si>
+  <si>
+    <t>(e10-6, 2)-differential privacy</t>
   </si>
 </sst>
 </file>
@@ -17017,6 +17020,907 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5A45-4CEC-93F2-2167459194C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1887996575"/>
+        <c:axId val="1887990751"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1024859584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1024860000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1024860000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1024859584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1887990751"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1887996575"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1887996575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1887990751"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(e10-6, 2)-Differential Privacy</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Global!$DG$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Global!$DG$2:$DG$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="0">
+                  <c:v>14491.666666666601</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12988.666666666601</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8285.3333333333303</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5897.3333333333303</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3673</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3368</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3049.6666666666601</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2616.3333333333298</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2422.3333333333298</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2321.6666666666601</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2306.6666666666601</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2279</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1795</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1706.3333333333301</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1665</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1865.6666666666599</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1740</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1876.3333333333301</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1677.6666666666599</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1437.6666666666599</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1449.6666666666599</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1578.3333333333301</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1522</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1450.3333333333301</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1420.6666666666599</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1849.6666666666599</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1522.3333333333301</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1780.3333333333301</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1535.3333333333301</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1369.6666666666599</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1831.3333333333301</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1765</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1877.3333333333301</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1898.3333333333301</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1903.6666666666599</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1922.6666666666599</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1974.3333333333301</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2235</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1890.3333333333301</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2218.3333333333298</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2399</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2424</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2144.6666666666601</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2373</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2353</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2356.6666666666601</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2625</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2684.3333333333298</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2590.6666666666601</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2614.6666666666601</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3197.6666666666601</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2881</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2844.6666666666601</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2831</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3017.3333333333298</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3047</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3090.3333333333298</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3650.3333333333298</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3961.3333333333298</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3170.3333333333298</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3987</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4315.3333333333303</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3FC6-4FA9-985E-4BEF24E613F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1024859584"/>
+        <c:axId val="1024860000"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Global!$DF$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Granularity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Global!$DF$2:$DF$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="0">
+                  <c:v>0.57176207514791</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.37556250031312199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26375253918106101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.193893698388903</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.162975858242282</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.131051319964998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11032479153902</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.7420120812517996E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.5710852707038196E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.3236523644779505E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.3259786463999407E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.6123009602124602E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.1667817358462903E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.6877206657495903E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.3843183471745602E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.1275807834952501E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.8972441400914798E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.6846850572282201E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.4733370374740197E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.2983606906646298E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.1547312444784301E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.0128818094769E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.89872329821491E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.7535990495283699E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.6499141892202E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5325819309356599E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.4286103599135599E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.32743710680769E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.2477336255262499E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.16907482548515E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.1068032418373499E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.05697137315899E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.0102818299256701E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.96363007504535E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.8990240563838801E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.8449366452834601E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.81568720983382E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.7538052254954101E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.68839474464762E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.64312136282087E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.5904808224680399E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.5351289604355301E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.489764732083E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.4591250242523101E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.39488654760552E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.3659510453351099E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.3250276550399001E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.2718450148090201E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.22943773909847E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.1853703292054599E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.1720661083289501E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.15140064657914E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.1168034578857899E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.08214451129728E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.0602900280165899E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.03678597064105E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.01419215999112E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>9.9043532782365409E-3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>9.7756146118165507E-3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>9.5593736977078892E-3</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>9.3463478959353898E-3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>9.1665729352990496E-3</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>8.9713526583480793E-3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>8.64932657338199E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3FC6-4FA9-985E-4BEF24E613F0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -24349,6 +25253,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors27.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -34044,6 +34988,529 @@
 </file>
 
 <file path=xl/charts/style26.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="325">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style27.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="325">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -39222,6 +40689,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>104</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>110</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Diagramm 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68449679-A9DB-44C2-9EF6-F191F55C676D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -39524,7 +41029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8959742-C5B8-4D5E-8EB1-1E24848E00F5}">
   <dimension ref="A1:CY65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -57414,15 +58919,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E08F581-ECA6-40F4-AA0A-73D637039F72}">
-  <dimension ref="A1:CY65"/>
+  <dimension ref="A1:DG65"/>
   <sheetViews>
-    <sheetView topLeftCell="CH1" workbookViewId="0">
-      <selection activeCell="CV27" sqref="CV27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -57696,8 +59201,29 @@
       <c r="CY1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="DA1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="DB1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="DC1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="DD1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="DE1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -57971,8 +59497,29 @@
       <c r="CY2" s="1">
         <v>670638.33333333302</v>
       </c>
+      <c r="DA2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE2" s="1">
+        <v>1</v>
+      </c>
+      <c r="DF2" s="1">
+        <v>0.57176207514791</v>
+      </c>
+      <c r="DG2" s="1">
+        <v>14491.666666666601</v>
+      </c>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -58246,8 +59793,29 @@
       <c r="CY3" s="1">
         <v>425335.66666666599</v>
       </c>
+      <c r="DA3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE3" s="1">
+        <v>2</v>
+      </c>
+      <c r="DF3" s="1">
+        <v>0.37556250031312199</v>
+      </c>
+      <c r="DG3" s="1">
+        <v>12988.666666666601</v>
+      </c>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -58521,8 +60089,29 @@
       <c r="CY4" s="1">
         <v>307363.33333333302</v>
       </c>
+      <c r="DA4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE4" s="1">
+        <v>3</v>
+      </c>
+      <c r="DF4" s="1">
+        <v>0.26375253918106101</v>
+      </c>
+      <c r="DG4" s="1">
+        <v>8285.3333333333303</v>
+      </c>
     </row>
-    <row r="5" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -58796,8 +60385,29 @@
       <c r="CY5" s="1">
         <v>211644</v>
       </c>
+      <c r="DA5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE5" s="1">
+        <v>4</v>
+      </c>
+      <c r="DF5" s="1">
+        <v>0.193893698388903</v>
+      </c>
+      <c r="DG5" s="1">
+        <v>5897.3333333333303</v>
+      </c>
     </row>
-    <row r="6" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -59071,8 +60681,29 @@
       <c r="CY6" s="1">
         <v>223424</v>
       </c>
+      <c r="DA6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE6" s="1">
+        <v>5</v>
+      </c>
+      <c r="DF6" s="1">
+        <v>0.162975858242282</v>
+      </c>
+      <c r="DG6" s="1">
+        <v>3673</v>
+      </c>
     </row>
-    <row r="7" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -59346,8 +60977,29 @@
       <c r="CY7" s="1">
         <v>209927.33333333299</v>
       </c>
+      <c r="DA7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE7" s="1">
+        <v>6</v>
+      </c>
+      <c r="DF7" s="1">
+        <v>0.131051319964998</v>
+      </c>
+      <c r="DG7" s="1">
+        <v>3368</v>
+      </c>
     </row>
-    <row r="8" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -59621,8 +61273,29 @@
       <c r="CY8" s="1">
         <v>191779.33333333299</v>
       </c>
+      <c r="DA8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE8" s="1">
+        <v>7</v>
+      </c>
+      <c r="DF8" s="1">
+        <v>0.11032479153902</v>
+      </c>
+      <c r="DG8" s="1">
+        <v>3049.6666666666601</v>
+      </c>
     </row>
-    <row r="9" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -59896,8 +61569,29 @@
       <c r="CY9" s="1">
         <v>151069.66666666599</v>
       </c>
+      <c r="DA9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE9" s="1">
+        <v>8</v>
+      </c>
+      <c r="DF9" s="1">
+        <v>9.7420120812517996E-2</v>
+      </c>
+      <c r="DG9" s="1">
+        <v>2616.3333333333298</v>
+      </c>
     </row>
-    <row r="10" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -60171,8 +61865,29 @@
       <c r="CY10" s="1">
         <v>154683.66666666599</v>
       </c>
+      <c r="DA10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE10" s="1">
+        <v>9</v>
+      </c>
+      <c r="DF10" s="1">
+        <v>8.5710852707038196E-2</v>
+      </c>
+      <c r="DG10" s="1">
+        <v>2422.3333333333298</v>
+      </c>
     </row>
-    <row r="11" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -60446,8 +62161,29 @@
       <c r="CY11" s="1">
         <v>151067.33333333299</v>
       </c>
+      <c r="DA11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE11" s="1">
+        <v>10</v>
+      </c>
+      <c r="DF11" s="1">
+        <v>7.3236523644779505E-2</v>
+      </c>
+      <c r="DG11" s="1">
+        <v>2321.6666666666601</v>
+      </c>
     </row>
-    <row r="12" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -60721,8 +62457,29 @@
       <c r="CY12" s="1">
         <v>144753</v>
       </c>
+      <c r="DA12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE12" s="1">
+        <v>11</v>
+      </c>
+      <c r="DF12" s="1">
+        <v>6.3259786463999407E-2</v>
+      </c>
+      <c r="DG12" s="1">
+        <v>2306.6666666666601</v>
+      </c>
     </row>
-    <row r="13" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -60996,8 +62753,29 @@
       <c r="CY13" s="1">
         <v>135302.33333333299</v>
       </c>
+      <c r="DA13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE13" s="1">
+        <v>12</v>
+      </c>
+      <c r="DF13" s="1">
+        <v>5.6123009602124602E-2</v>
+      </c>
+      <c r="DG13" s="1">
+        <v>2004</v>
+      </c>
     </row>
-    <row r="14" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -61271,8 +63049,29 @@
       <c r="CY14" s="1">
         <v>126883.666666666</v>
       </c>
+      <c r="DA14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE14" s="1">
+        <v>13</v>
+      </c>
+      <c r="DF14" s="1">
+        <v>5.1667817358462903E-2</v>
+      </c>
+      <c r="DG14" s="1">
+        <v>2279</v>
+      </c>
     </row>
-    <row r="15" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -61546,8 +63345,29 @@
       <c r="CY15" s="1">
         <v>120552.666666666</v>
       </c>
+      <c r="DA15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE15" s="1">
+        <v>14</v>
+      </c>
+      <c r="DF15" s="1">
+        <v>4.6877206657495903E-2</v>
+      </c>
+      <c r="DG15" s="1">
+        <v>1795</v>
+      </c>
     </row>
-    <row r="16" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -61821,8 +63641,29 @@
       <c r="CY16" s="1">
         <v>117945</v>
       </c>
+      <c r="DA16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE16" s="1">
+        <v>15</v>
+      </c>
+      <c r="DF16" s="1">
+        <v>4.3843183471745602E-2</v>
+      </c>
+      <c r="DG16" s="1">
+        <v>1706.3333333333301</v>
+      </c>
     </row>
-    <row r="17" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -62096,8 +63937,29 @@
       <c r="CY17" s="1">
         <v>126079.666666666</v>
       </c>
+      <c r="DA17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE17" s="1">
+        <v>16</v>
+      </c>
+      <c r="DF17" s="1">
+        <v>4.1275807834952501E-2</v>
+      </c>
+      <c r="DG17" s="1">
+        <v>1665</v>
+      </c>
     </row>
-    <row r="18" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -62371,8 +64233,29 @@
       <c r="CY18" s="1">
         <v>113138</v>
       </c>
+      <c r="DA18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE18" s="1">
+        <v>17</v>
+      </c>
+      <c r="DF18" s="1">
+        <v>3.8972441400914798E-2</v>
+      </c>
+      <c r="DG18" s="1">
+        <v>1865.6666666666599</v>
+      </c>
     </row>
-    <row r="19" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -62646,8 +64529,29 @@
       <c r="CY19" s="1">
         <v>116513.33333333299</v>
       </c>
+      <c r="DA19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE19" s="1">
+        <v>18</v>
+      </c>
+      <c r="DF19" s="1">
+        <v>3.6846850572282201E-2</v>
+      </c>
+      <c r="DG19" s="1">
+        <v>1740</v>
+      </c>
     </row>
-    <row r="20" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -62921,8 +64825,29 @@
       <c r="CY20" s="1">
         <v>102858.33333333299</v>
       </c>
+      <c r="DA20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE20" s="1">
+        <v>19</v>
+      </c>
+      <c r="DF20" s="1">
+        <v>3.4733370374740197E-2</v>
+      </c>
+      <c r="DG20" s="1">
+        <v>1876.3333333333301</v>
+      </c>
     </row>
-    <row r="21" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -63196,8 +65121,29 @@
       <c r="CY21" s="1">
         <v>100355</v>
       </c>
+      <c r="DA21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE21" s="1">
+        <v>20</v>
+      </c>
+      <c r="DF21" s="1">
+        <v>3.2983606906646298E-2</v>
+      </c>
+      <c r="DG21" s="1">
+        <v>1677.6666666666599</v>
+      </c>
     </row>
-    <row r="22" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -63471,8 +65417,29 @@
       <c r="CY22" s="1">
         <v>97103</v>
       </c>
+      <c r="DA22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE22" s="1">
+        <v>21</v>
+      </c>
+      <c r="DF22" s="1">
+        <v>3.1547312444784301E-2</v>
+      </c>
+      <c r="DG22" s="1">
+        <v>1437.6666666666599</v>
+      </c>
     </row>
-    <row r="23" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -63746,8 +65713,29 @@
       <c r="CY23" s="1">
         <v>95964.333333333299</v>
       </c>
+      <c r="DA23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE23" s="1">
+        <v>22</v>
+      </c>
+      <c r="DF23" s="1">
+        <v>3.0128818094769E-2</v>
+      </c>
+      <c r="DG23" s="1">
+        <v>1449.6666666666599</v>
+      </c>
     </row>
-    <row r="24" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -64021,8 +66009,29 @@
       <c r="CY24" s="1">
         <v>93373</v>
       </c>
+      <c r="DA24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE24" s="1">
+        <v>23</v>
+      </c>
+      <c r="DF24" s="1">
+        <v>2.89872329821491E-2</v>
+      </c>
+      <c r="DG24" s="1">
+        <v>1578.3333333333301</v>
+      </c>
     </row>
-    <row r="25" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -64296,8 +66305,29 @@
       <c r="CY25" s="1">
         <v>94310.666666666599</v>
       </c>
+      <c r="DA25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE25" s="1">
+        <v>24</v>
+      </c>
+      <c r="DF25" s="1">
+        <v>2.7535990495283699E-2</v>
+      </c>
+      <c r="DG25" s="1">
+        <v>1522</v>
+      </c>
     </row>
-    <row r="26" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -64571,8 +66601,29 @@
       <c r="CY26" s="1">
         <v>86687</v>
       </c>
+      <c r="DA26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE26" s="1">
+        <v>25</v>
+      </c>
+      <c r="DF26" s="1">
+        <v>2.6499141892202E-2</v>
+      </c>
+      <c r="DG26" s="1">
+        <v>1450.3333333333301</v>
+      </c>
     </row>
-    <row r="27" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -64846,8 +66897,29 @@
       <c r="CY27" s="1">
         <v>86814</v>
       </c>
+      <c r="DA27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE27" s="1">
+        <v>26</v>
+      </c>
+      <c r="DF27" s="1">
+        <v>2.5325819309356599E-2</v>
+      </c>
+      <c r="DG27" s="1">
+        <v>1420.6666666666599</v>
+      </c>
     </row>
-    <row r="28" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -65121,8 +67193,29 @@
       <c r="CY28" s="1">
         <v>81584.666666666599</v>
       </c>
+      <c r="DA28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE28" s="1">
+        <v>27</v>
+      </c>
+      <c r="DF28" s="1">
+        <v>2.4286103599135599E-2</v>
+      </c>
+      <c r="DG28" s="1">
+        <v>1849.6666666666599</v>
+      </c>
     </row>
-    <row r="29" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
@@ -65396,8 +67489,29 @@
       <c r="CY29" s="1">
         <v>79801.666666666599</v>
       </c>
+      <c r="DA29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE29" s="1">
+        <v>28</v>
+      </c>
+      <c r="DF29" s="1">
+        <v>2.32743710680769E-2</v>
+      </c>
+      <c r="DG29" s="1">
+        <v>1522.3333333333301</v>
+      </c>
     </row>
-    <row r="30" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -65671,8 +67785,29 @@
       <c r="CY30" s="1">
         <v>80503.333333333299</v>
       </c>
+      <c r="DA30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE30" s="1">
+        <v>29</v>
+      </c>
+      <c r="DF30" s="1">
+        <v>2.2477336255262499E-2</v>
+      </c>
+      <c r="DG30" s="1">
+        <v>1780.3333333333301</v>
+      </c>
     </row>
-    <row r="31" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -65946,8 +68081,29 @@
       <c r="CY31" s="1">
         <v>76535.666666666599</v>
       </c>
+      <c r="DA31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE31" s="1">
+        <v>30</v>
+      </c>
+      <c r="DF31" s="1">
+        <v>2.16907482548515E-2</v>
+      </c>
+      <c r="DG31" s="1">
+        <v>1535.3333333333301</v>
+      </c>
     </row>
-    <row r="32" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -66221,8 +68377,29 @@
       <c r="CY32" s="1">
         <v>76620.666666666599</v>
       </c>
+      <c r="DA32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE32" s="1">
+        <v>31</v>
+      </c>
+      <c r="DF32" s="1">
+        <v>2.1068032418373499E-2</v>
+      </c>
+      <c r="DG32" s="1">
+        <v>1369.6666666666599</v>
+      </c>
     </row>
-    <row r="33" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -66496,8 +68673,29 @@
       <c r="CY33" s="1">
         <v>74659</v>
       </c>
+      <c r="DA33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE33" s="1">
+        <v>32</v>
+      </c>
+      <c r="DF33" s="1">
+        <v>2.05697137315899E-2</v>
+      </c>
+      <c r="DG33" s="1">
+        <v>1831.3333333333301</v>
+      </c>
     </row>
-    <row r="34" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -66771,8 +68969,29 @@
       <c r="CY34" s="1">
         <v>77506.333333333299</v>
       </c>
+      <c r="DA34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE34" s="1">
+        <v>33</v>
+      </c>
+      <c r="DF34" s="1">
+        <v>2.0102818299256701E-2</v>
+      </c>
+      <c r="DG34" s="1">
+        <v>1765</v>
+      </c>
     </row>
-    <row r="35" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
@@ -67046,8 +69265,29 @@
       <c r="CY35" s="1">
         <v>76638.666666666599</v>
       </c>
+      <c r="DA35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE35" s="1">
+        <v>34</v>
+      </c>
+      <c r="DF35" s="1">
+        <v>1.96363007504535E-2</v>
+      </c>
+      <c r="DG35" s="1">
+        <v>1877.3333333333301</v>
+      </c>
     </row>
-    <row r="36" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -67321,8 +69561,29 @@
       <c r="CY36" s="1">
         <v>77621</v>
       </c>
+      <c r="DA36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE36" s="1">
+        <v>35</v>
+      </c>
+      <c r="DF36" s="1">
+        <v>1.8990240563838801E-2</v>
+      </c>
+      <c r="DG36" s="1">
+        <v>1898.3333333333301</v>
+      </c>
     </row>
-    <row r="37" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -67596,8 +69857,29 @@
       <c r="CY37" s="1">
         <v>70115</v>
       </c>
+      <c r="DA37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE37" s="1">
+        <v>36</v>
+      </c>
+      <c r="DF37" s="1">
+        <v>1.8449366452834601E-2</v>
+      </c>
+      <c r="DG37" s="1">
+        <v>2026</v>
+      </c>
     </row>
-    <row r="38" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
@@ -67871,8 +70153,29 @@
       <c r="CY38" s="1">
         <v>68227.333333333299</v>
       </c>
+      <c r="DA38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE38" s="1">
+        <v>37</v>
+      </c>
+      <c r="DF38" s="1">
+        <v>1.81568720983382E-2</v>
+      </c>
+      <c r="DG38" s="1">
+        <v>1903.6666666666599</v>
+      </c>
     </row>
-    <row r="39" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
@@ -68146,8 +70449,29 @@
       <c r="CY39" s="1">
         <v>71823.333333333299</v>
       </c>
+      <c r="DA39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE39" s="1">
+        <v>38</v>
+      </c>
+      <c r="DF39" s="1">
+        <v>1.7538052254954101E-2</v>
+      </c>
+      <c r="DG39" s="1">
+        <v>1922.6666666666599</v>
+      </c>
     </row>
-    <row r="40" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
@@ -68421,8 +70745,29 @@
       <c r="CY40" s="1">
         <v>63901</v>
       </c>
+      <c r="DA40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE40" s="1">
+        <v>39</v>
+      </c>
+      <c r="DF40" s="1">
+        <v>1.68839474464762E-2</v>
+      </c>
+      <c r="DG40" s="1">
+        <v>1974.3333333333301</v>
+      </c>
     </row>
-    <row r="41" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
@@ -68696,8 +71041,29 @@
       <c r="CY41" s="1">
         <v>61193.333333333299</v>
       </c>
+      <c r="DA41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE41" s="1">
+        <v>40</v>
+      </c>
+      <c r="DF41" s="1">
+        <v>1.64312136282087E-2</v>
+      </c>
+      <c r="DG41" s="1">
+        <v>2235</v>
+      </c>
     </row>
-    <row r="42" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
@@ -68971,8 +71337,29 @@
       <c r="CY42" s="1">
         <v>62458.333333333299</v>
       </c>
+      <c r="DA42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE42" s="1">
+        <v>41</v>
+      </c>
+      <c r="DF42" s="1">
+        <v>1.5904808224680399E-2</v>
+      </c>
+      <c r="DG42" s="1">
+        <v>1890.3333333333301</v>
+      </c>
     </row>
-    <row r="43" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
@@ -69246,8 +71633,29 @@
       <c r="CY43" s="1">
         <v>58789.333333333299</v>
       </c>
+      <c r="DA43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE43" s="1">
+        <v>42</v>
+      </c>
+      <c r="DF43" s="1">
+        <v>1.5351289604355301E-2</v>
+      </c>
+      <c r="DG43" s="1">
+        <v>2218.3333333333298</v>
+      </c>
     </row>
-    <row r="44" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
@@ -69521,8 +71929,29 @@
       <c r="CY44" s="1">
         <v>64234</v>
       </c>
+      <c r="DA44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB44" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE44" s="1">
+        <v>43</v>
+      </c>
+      <c r="DF44" s="1">
+        <v>1.489764732083E-2</v>
+      </c>
+      <c r="DG44" s="1">
+        <v>2399</v>
+      </c>
     </row>
-    <row r="45" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
@@ -69796,8 +72225,29 @@
       <c r="CY45" s="1">
         <v>62876</v>
       </c>
+      <c r="DA45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE45" s="1">
+        <v>44</v>
+      </c>
+      <c r="DF45" s="1">
+        <v>1.4591250242523101E-2</v>
+      </c>
+      <c r="DG45" s="1">
+        <v>2424</v>
+      </c>
     </row>
-    <row r="46" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -70071,8 +72521,29 @@
       <c r="CY46" s="1">
         <v>64067</v>
       </c>
+      <c r="DA46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE46" s="1">
+        <v>45</v>
+      </c>
+      <c r="DF46" s="1">
+        <v>1.39488654760552E-2</v>
+      </c>
+      <c r="DG46" s="1">
+        <v>2144.6666666666601</v>
+      </c>
     </row>
-    <row r="47" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>7</v>
       </c>
@@ -70346,8 +72817,29 @@
       <c r="CY47" s="1">
         <v>64083</v>
       </c>
+      <c r="DA47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB47" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE47" s="1">
+        <v>46</v>
+      </c>
+      <c r="DF47" s="1">
+        <v>1.3659510453351099E-2</v>
+      </c>
+      <c r="DG47" s="1">
+        <v>2373</v>
+      </c>
     </row>
-    <row r="48" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
@@ -70621,8 +73113,29 @@
       <c r="CY48" s="1">
         <v>64719</v>
       </c>
+      <c r="DA48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE48" s="1">
+        <v>47</v>
+      </c>
+      <c r="DF48" s="1">
+        <v>1.3250276550399001E-2</v>
+      </c>
+      <c r="DG48" s="1">
+        <v>2353</v>
+      </c>
     </row>
-    <row r="49" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
@@ -70896,8 +73409,29 @@
       <c r="CY49" s="1">
         <v>60777.333333333299</v>
       </c>
+      <c r="DA49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE49" s="1">
+        <v>48</v>
+      </c>
+      <c r="DF49" s="1">
+        <v>1.2718450148090201E-2</v>
+      </c>
+      <c r="DG49" s="1">
+        <v>2356.6666666666601</v>
+      </c>
     </row>
-    <row r="50" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -71171,8 +73705,29 @@
       <c r="CY50" s="1">
         <v>60705.666666666599</v>
       </c>
+      <c r="DA50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE50" s="1">
+        <v>49</v>
+      </c>
+      <c r="DF50" s="1">
+        <v>1.22943773909847E-2</v>
+      </c>
+      <c r="DG50" s="1">
+        <v>2625</v>
+      </c>
     </row>
-    <row r="51" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -71446,8 +74001,29 @@
       <c r="CY51" s="1">
         <v>55443.333333333299</v>
       </c>
+      <c r="DA51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE51" s="1">
+        <v>50</v>
+      </c>
+      <c r="DF51" s="1">
+        <v>1.1853703292054599E-2</v>
+      </c>
+      <c r="DG51" s="1">
+        <v>2684.3333333333298</v>
+      </c>
     </row>
-    <row r="52" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -71721,8 +74297,29 @@
       <c r="CY52" s="1">
         <v>55929</v>
       </c>
+      <c r="DA52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE52" s="1">
+        <v>51</v>
+      </c>
+      <c r="DF52" s="1">
+        <v>1.1720661083289501E-2</v>
+      </c>
+      <c r="DG52" s="1">
+        <v>2590.6666666666601</v>
+      </c>
     </row>
-    <row r="53" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
@@ -71996,8 +74593,29 @@
       <c r="CY53" s="1">
         <v>56691</v>
       </c>
+      <c r="DA53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE53" s="1">
+        <v>52</v>
+      </c>
+      <c r="DF53" s="1">
+        <v>1.15140064657914E-2</v>
+      </c>
+      <c r="DG53" s="1">
+        <v>2614.6666666666601</v>
+      </c>
     </row>
-    <row r="54" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
@@ -72271,8 +74889,29 @@
       <c r="CY54" s="1">
         <v>54188.666666666599</v>
       </c>
+      <c r="DA54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE54" s="1">
+        <v>53</v>
+      </c>
+      <c r="DF54" s="1">
+        <v>1.1168034578857899E-2</v>
+      </c>
+      <c r="DG54" s="1">
+        <v>3197.6666666666601</v>
+      </c>
     </row>
-    <row r="55" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>7</v>
       </c>
@@ -72546,8 +75185,29 @@
       <c r="CY55" s="1">
         <v>52333.333333333299</v>
       </c>
+      <c r="DA55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE55" s="1">
+        <v>54</v>
+      </c>
+      <c r="DF55" s="1">
+        <v>1.08214451129728E-2</v>
+      </c>
+      <c r="DG55" s="1">
+        <v>2881</v>
+      </c>
     </row>
-    <row r="56" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -72821,8 +75481,29 @@
       <c r="CY56" s="1">
         <v>51040.666666666599</v>
       </c>
+      <c r="DA56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE56" s="1">
+        <v>55</v>
+      </c>
+      <c r="DF56" s="1">
+        <v>1.0602900280165899E-2</v>
+      </c>
+      <c r="DG56" s="1">
+        <v>2844.6666666666601</v>
+      </c>
     </row>
-    <row r="57" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -73096,8 +75777,29 @@
       <c r="CY57" s="1">
         <v>60952.333333333299</v>
       </c>
+      <c r="DA57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE57" s="1">
+        <v>56</v>
+      </c>
+      <c r="DF57" s="1">
+        <v>1.03678597064105E-2</v>
+      </c>
+      <c r="DG57" s="1">
+        <v>2831</v>
+      </c>
     </row>
-    <row r="58" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -73371,8 +76073,29 @@
       <c r="CY58" s="1">
         <v>54645.666666666599</v>
       </c>
+      <c r="DA58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE58" s="1">
+        <v>57</v>
+      </c>
+      <c r="DF58" s="1">
+        <v>1.01419215999112E-2</v>
+      </c>
+      <c r="DG58" s="1">
+        <v>3017.3333333333298</v>
+      </c>
     </row>
-    <row r="59" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
@@ -73646,8 +76369,29 @@
       <c r="CY59" s="1">
         <v>54550</v>
       </c>
+      <c r="DA59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE59" s="1">
+        <v>58</v>
+      </c>
+      <c r="DF59" s="1">
+        <v>9.9043532782365409E-3</v>
+      </c>
+      <c r="DG59" s="1">
+        <v>3047</v>
+      </c>
     </row>
-    <row r="60" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -73921,8 +76665,29 @@
       <c r="CY60" s="1">
         <v>56603.666666666599</v>
       </c>
+      <c r="DA60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE60" s="1">
+        <v>59</v>
+      </c>
+      <c r="DF60" s="1">
+        <v>9.7756146118165507E-3</v>
+      </c>
+      <c r="DG60" s="1">
+        <v>3090.3333333333298</v>
+      </c>
     </row>
-    <row r="61" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -74196,8 +76961,29 @@
       <c r="CY61" s="1">
         <v>56941.666666666599</v>
       </c>
+      <c r="DA61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE61" s="1">
+        <v>60</v>
+      </c>
+      <c r="DF61" s="1">
+        <v>9.5593736977078892E-3</v>
+      </c>
+      <c r="DG61" s="1">
+        <v>3650.3333333333298</v>
+      </c>
     </row>
-    <row r="62" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -74471,8 +77257,29 @@
       <c r="CY62" s="1">
         <v>53731.333333333299</v>
       </c>
+      <c r="DA62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB62" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE62" s="1">
+        <v>61</v>
+      </c>
+      <c r="DF62" s="1">
+        <v>9.3463478959353898E-3</v>
+      </c>
+      <c r="DG62" s="1">
+        <v>3961.3333333333298</v>
+      </c>
     </row>
-    <row r="63" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -74746,8 +77553,29 @@
       <c r="CY63" s="1">
         <v>55666</v>
       </c>
+      <c r="DA63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB63" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD63" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE63" s="1">
+        <v>62</v>
+      </c>
+      <c r="DF63" s="1">
+        <v>9.1665729352990496E-3</v>
+      </c>
+      <c r="DG63" s="1">
+        <v>3170.3333333333298</v>
+      </c>
     </row>
-    <row r="64" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -75021,8 +77849,29 @@
       <c r="CY64" s="1">
         <v>51396.333333333299</v>
       </c>
+      <c r="DA64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB64" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE64" s="1">
+        <v>63</v>
+      </c>
+      <c r="DF64" s="1">
+        <v>8.9713526583480793E-3</v>
+      </c>
+      <c r="DG64" s="1">
+        <v>3987</v>
+      </c>
     </row>
-    <row r="65" spans="1:103" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -75295,6 +78144,27 @@
       </c>
       <c r="CY65" s="1">
         <v>51306</v>
+      </c>
+      <c r="DA65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DB65" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DC65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DD65" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE65" s="1">
+        <v>64</v>
+      </c>
+      <c r="DF65" s="1">
+        <v>8.64932657338199E-3</v>
+      </c>
+      <c r="DG65" s="1">
+        <v>4315.3333333333303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>